<commit_message>
- Pflichtenheft aktualisiert - Projektkosten aktualisiert
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/Definition/Projektkosten_PAMS_Verteilt.xlsx
+++ b/documents/projectmanagement/Definition/Projektkosten_PAMS_Verteilt.xlsx
@@ -70,19 +70,7 @@
     <t>Berater</t>
   </si>
   <si>
-    <t>32h, Machbarkeit, Umfeld, Risiko</t>
-  </si>
-  <si>
-    <t>40h, Konzeption, Dokumenation</t>
-  </si>
-  <si>
     <t>30h, Design Entwurf, Umsetzung, Anpassung</t>
-  </si>
-  <si>
-    <t>8h, DB-Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25h, PHP-DB, PHP-Logik  </t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -148,6 +136,18 @@
   </si>
   <si>
     <t>4h, durch Techniker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25h, Logik, Ausgabe, Eingabe, Datenbankzugriff, Login(Verschlüsselung), </t>
+  </si>
+  <si>
+    <t>8h, DB-Design, Erstellung</t>
+  </si>
+  <si>
+    <t>40h, Konzeption, Dokumenation, Aufgabenverteilung, Budgetverwaltung, Meilensteine festlegen</t>
+  </si>
+  <si>
+    <t>32h, Machbarkeit, Umfeld, Risiko, Statusberichte, Kommunikationsrichtlinien, Dokumentationsrichtlinien</t>
   </si>
 </sst>
 </file>
@@ -244,7 +244,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -255,10 +255,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1"/>
@@ -274,6 +270,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -587,8 +592,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,18 +604,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -625,55 +630,55 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <f>30*55</f>
         <v>1650</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>8050</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="8">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6">
         <f>2*116.85</f>
         <v>233.7</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="10">
         <f>SUM(B4:B6)</f>
         <v>9933.7000000000007</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -688,31 +693,31 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="8">
+        <v>38</v>
+      </c>
+      <c r="B10" s="6">
         <v>480</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="10">
+      <c r="A11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8">
         <f>SUM(B10)</f>
         <v>480</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -725,82 +730,82 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>23</v>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>681.6</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="16">
         <v>4368</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>2238</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="16">
         <v>3417.6</v>
       </c>
-      <c r="C18" t="s">
-        <v>18</v>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <f>(SUM(B14:B18))*0.05</f>
         <v>535.2600000000001</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="10">
+      <c r="A20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="8">
         <f>SUM(B14:B19)</f>
         <v>11240.460000000001</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -843,14 +848,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="12">
+      <c r="A25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="10">
         <f>SUM(B23:B24)</f>
         <v>160</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -872,24 +877,24 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>800</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="A29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="10">
         <f>SUM(B28)</f>
         <v>800</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -910,20 +915,20 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="12">
+      <c r="A32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10">
         <v>0</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10">
+      <c r="A33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8">
         <f>B20+B25+B29+B32+B11+B7</f>
         <v>22614.160000000003</v>
       </c>

</xml_diff>